<commit_message>
remove bload add style
</commit_message>
<xml_diff>
--- a/rdqe.xlsx
+++ b/rdqe.xlsx
@@ -451,7 +451,7 @@
         <v>S723E</v>
       </c>
       <c r="B2" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C2" t="str">
         <v>95,62</v>
@@ -492,7 +492,7 @@
         <v>EBBL</v>
       </c>
       <c r="B3" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C3" t="str">
         <v>-</v>
@@ -533,7 +533,7 @@
         <v>GEEK</v>
       </c>
       <c r="B4" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C4" t="str">
         <v>95,28</v>
@@ -574,7 +574,7 @@
         <v>EBFS</v>
       </c>
       <c r="B5" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C5" t="str">
         <v>93,21</v>
@@ -615,7 +615,7 @@
         <v>EBSH</v>
       </c>
       <c r="B6" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C6" t="str">
         <v/>
@@ -656,7 +656,7 @@
         <v>EBBE</v>
       </c>
       <c r="B7" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C7" t="str">
         <v/>
@@ -697,7 +697,7 @@
         <v>GEMB</v>
       </c>
       <c r="B8" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C8" t="str">
         <v/>
@@ -741,7 +741,7 @@
         <v>EBEZ</v>
       </c>
       <c r="B9" t="str">
-        <v>2020202</v>
+        <v>test</v>
       </c>
       <c r="C9" t="str">
         <v/>

</xml_diff>